<commit_message>
Modifs post pause. bugs modifs effacees
</commit_message>
<xml_diff>
--- a/asset/diagram.xlsx
+++ b/asset/diagram.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/formateur/Desktop/jeu_de_paires/asset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A46F042-2CE9-E842-BE1A-9A78E71FC956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309F6355-05D2-9E48-BA57-0283E9A880B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="500" windowWidth="25600" windowHeight="13900" xr2:uid="{8735055C-E134-3E4D-82DA-80B73531BE17}"/>
+    <workbookView xWindow="-25600" yWindow="2620" windowWidth="25600" windowHeight="13900" xr2:uid="{8735055C-E134-3E4D-82DA-80B73531BE17}"/>
   </bookViews>
   <sheets>
     <sheet name="Diagram" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>dataSource</t>
   </si>
@@ -245,9 +245,6 @@
     <t>Malac</t>
   </si>
   <si>
-    <t>Armede</t>
-  </si>
-  <si>
     <t>Kali</t>
   </si>
   <si>
@@ -264,7 +261,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -283,6 +280,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -459,11 +463,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -496,6 +499,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -981,8 +987,8 @@
   </sheetPr>
   <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -999,270 +1005,270 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="20"/>
-      <c r="J1" s="18" t="s">
+      <c r="G1" s="18"/>
+      <c r="H1" s="19"/>
+      <c r="J1" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="19"/>
-      <c r="L1" s="20"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="19"/>
     </row>
     <row r="2" spans="3:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F2" s="12" t="str">
+      <c r="F2" s="11" t="str">
         <f>Param!A1</f>
         <v>Properties / Methods</v>
       </c>
-      <c r="G2" s="12" t="str">
+      <c r="G2" s="11" t="str">
         <f>Param!A2</f>
         <v>Description</v>
       </c>
-      <c r="H2" s="12" t="str">
+      <c r="H2" s="11" t="str">
         <f>Param!A3</f>
         <v>Assignment</v>
       </c>
-      <c r="J2" s="12" t="str">
+      <c r="J2" s="11" t="str">
         <f>Param!A1</f>
         <v>Properties / Methods</v>
       </c>
-      <c r="K2" s="12" t="str">
+      <c r="K2" s="11" t="str">
         <f>Param!A2</f>
         <v>Description</v>
       </c>
-      <c r="L2" s="13" t="str">
+      <c r="L2" s="12" t="str">
         <f>Param!A3</f>
         <v>Assignment</v>
       </c>
     </row>
     <row r="3" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="J3" s="10" t="s">
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="J3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="10"/>
-      <c r="L3" s="8"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="7"/>
     </row>
     <row r="4" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="16"/>
-      <c r="J4" s="16" t="s">
+      <c r="H4" s="15"/>
+      <c r="J4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="16"/>
-      <c r="L4" s="17"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="16"/>
     </row>
     <row r="5" spans="3:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="J5" s="11" t="s">
+      <c r="H5" s="9"/>
+      <c r="J5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="K5" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="L5" s="9"/>
+      <c r="L5" s="8"/>
     </row>
     <row r="6" spans="3:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="11"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="8" spans="3:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="3:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="23"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="22"/>
     </row>
     <row r="10" spans="3:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="5" t="str">
+      <c r="C10" s="4" t="str">
         <f>Param!A1</f>
         <v>Properties / Methods</v>
       </c>
-      <c r="D10" s="5" t="str">
+      <c r="D10" s="4" t="str">
         <f>Param!A2</f>
         <v>Description</v>
       </c>
-      <c r="E10" s="4" t="str">
+      <c r="E10" s="3" t="str">
         <f>Param!A3</f>
         <v>Assignment</v>
       </c>
     </row>
     <row r="11" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="6"/>
+      <c r="D11" s="5"/>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="6"/>
+      <c r="D12" s="5"/>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="3:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="6"/>
+      <c r="D13" s="5"/>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="3:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="6"/>
+      <c r="D14" s="5"/>
       <c r="E14" s="2"/>
-      <c r="J14" s="18" t="s">
+      <c r="J14" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="K14" s="19"/>
-      <c r="L14" s="20"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="19"/>
     </row>
     <row r="15" spans="3:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="6"/>
+      <c r="D15" s="5"/>
       <c r="E15" s="2"/>
-      <c r="J15" s="12" t="str">
+      <c r="J15" s="11" t="str">
         <f>Param!A1</f>
         <v>Properties / Methods</v>
       </c>
-      <c r="K15" s="12" t="str">
+      <c r="K15" s="11" t="str">
         <f>Param!A2</f>
         <v>Description</v>
       </c>
-      <c r="L15" s="12" t="str">
+      <c r="L15" s="11" t="str">
         <f>Param!A3</f>
         <v>Assignment</v>
       </c>
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="15"/>
-      <c r="J16" s="10" t="s">
+      <c r="D16" s="13"/>
+      <c r="E16" s="14"/>
+      <c r="J16" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="K16" s="10" t="s">
+      <c r="K16" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L16" s="10"/>
+      <c r="L16" s="9"/>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>22</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="J17" s="10" t="s">
+      <c r="J17" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="K17" s="10" t="s">
+      <c r="K17" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="L17" s="10"/>
+      <c r="L17" s="9"/>
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="6"/>
+      <c r="D18" s="5"/>
       <c r="E18" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J18" s="16" t="s">
+      <c r="J18" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="K18" s="16" t="s">
+      <c r="K18" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="L18" s="16"/>
+      <c r="L18" s="15"/>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="J19" s="10" t="s">
+      <c r="J19" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="K19" s="10" t="s">
+      <c r="K19" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="L19" s="10" t="s">
+      <c r="L19" s="25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="K20" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="L20" s="10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="3:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J20" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="K20" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="L20" s="11" t="s">
-        <v>57</v>
-      </c>
-    </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="24" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="5" t="s">
         <v>30</v>
       </c>
       <c r="E22" s="2" t="s">
@@ -1270,10 +1276,10 @@
       </c>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="5" t="s">
         <v>29</v>
       </c>
       <c r="E23" s="2" t="s">
@@ -1281,19 +1287,19 @@
       </c>
     </row>
     <row r="24" spans="3:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>55</v>
+      <c r="E24" s="23" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.2">
       <c r="G28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>